<commit_message>
Modificaciones en la revision de columnas
</commit_message>
<xml_diff>
--- a/codigo/01-preprocesamiento-de-datos/Columnas_Dataset_Pisos.xlsx
+++ b/codigo/01-preprocesamiento-de-datos/Columnas_Dataset_Pisos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\extas\Documents\GitHub\precios-de-vivienda-madrid\codigo\01-preprocesamiento-de-datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BADEFEA-FA16-41F7-B97D-88F27D19FBDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FF6B11F-7E19-4710-9F55-DE694A0B0A7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -87,7 +87,127 @@
         </r>
       </text>
     </comment>
+    <comment ref="B88" authorId="1" shapeId="0" xr:uid="{3C7EE77E-6542-4C2D-B689-4E9E70376F8D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Silvia Gonzalez:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+tiene el valor exterior</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="C101" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>======
+ID#AAABb4BQ9t8
+Silvia Gonzalez    (2025-01-18 15:05:35)
+la hago yo que tengo tambien cocina</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C102" authorId="0" shapeId="0" xr:uid="{2451DF93-DB86-4A1F-B070-657D45C11300}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>======
+ID#AAABb4BQ9t8
+Silvia Gonzalez    (2025-01-18 15:05:35)
+la hago yo que tengo tambien cocina</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C103" authorId="0" shapeId="0" xr:uid="{586B480B-DB5B-41B7-8426-49D113623992}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>======
+ID#AAABb4BQ9t8
+Silvia Gonzalez    (2025-01-18 15:05:35)
+la hago yo que tengo tambien cocina</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C104" authorId="0" shapeId="0" xr:uid="{22E153EF-1BB5-4E1A-BA39-B45D210051F8}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>======
+ID#AAABb4BQ9t8
+Silvia Gonzalez    (2025-01-18 15:05:35)
+la hago yo que tengo tambien cocina</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C105" authorId="0" shapeId="0" xr:uid="{64243220-8DC2-4D16-92C5-BCBD854F1245}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>======
+ID#AAABb4BQ9t8
+Silvia Gonzalez    (2025-01-18 15:05:35)
+la hago yo que tengo tambien cocina</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C106" authorId="0" shapeId="0" xr:uid="{5E8DD8F2-E395-42BB-A942-78B04F004BF2}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>======
+ID#AAABb4BQ9t8
+Silvia Gonzalez    (2025-01-18 15:05:35)
+la hago yo que tengo tambien cocina</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C107" authorId="0" shapeId="0" xr:uid="{BD3125B6-6370-4A3C-A727-24F3B83BC206}">
       <text>
         <r>
           <rPr>
@@ -113,7 +233,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="355">
   <si>
     <t>orden_dataframe</t>
   </si>
@@ -1368,6 +1488,24 @@
   </si>
   <si>
     <t>1,0,nan (ver si lo juntamos con el tipo que es señorial, economica,…)</t>
+  </si>
+  <si>
+    <t>eliminar y poner los valores en €_comunidad_mes</t>
+  </si>
+  <si>
+    <t>En redpiso se quitaron las comas por lo que valores como 20,00 aparece ahora como 2000, hay que dividir entre 100 todos los valores</t>
+  </si>
+  <si>
+    <t>valores muy dispares, ir al origen de estos valores pisos.com para ver que hacer</t>
+  </si>
+  <si>
+    <t>los nan -1?</t>
+  </si>
+  <si>
+    <t>Exterior</t>
+  </si>
+  <si>
+    <t>eliminarla por que pondremos sus valores en la columna exterior</t>
   </si>
 </sst>
 </file>
@@ -1564,13 +1702,15 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1831,10 +1971,10 @@
   <dimension ref="A1:K1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F58" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C85" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A68" sqref="A68:XFD68"/>
+      <selection pane="bottomRight" activeCell="D113" sqref="D113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -3764,7 +3904,7 @@
       <c r="H63" s="10" t="s">
         <v>341</v>
       </c>
-      <c r="I63" s="23" t="s">
+      <c r="I63" t="s">
         <v>160</v>
       </c>
       <c r="J63" t="s">
@@ -3911,6 +4051,12 @@
       <c r="H69" s="8" t="s">
         <v>272</v>
       </c>
+      <c r="I69" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="J69" s="8" t="s">
+        <v>349</v>
+      </c>
     </row>
     <row r="70" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A70" s="7">
@@ -3920,7 +4066,7 @@
         <v>273</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>274</v>
+        <v>163</v>
       </c>
       <c r="D70" s="8"/>
       <c r="E70" s="8" t="s">
@@ -3944,7 +4090,7 @@
         <v>276</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>274</v>
+        <v>163</v>
       </c>
       <c r="D71" s="8"/>
       <c r="E71" s="8" t="s">
@@ -4027,6 +4173,12 @@
       <c r="H74" s="5" t="s">
         <v>287</v>
       </c>
+      <c r="J74" s="24" t="s">
+        <v>190</v>
+      </c>
+      <c r="K74" s="24" t="s">
+        <v>352</v>
+      </c>
     </row>
     <row r="75" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A75" s="7">
@@ -4054,7 +4206,7 @@
       <c r="I75" s="9" t="s">
         <v>289</v>
       </c>
-      <c r="J75" s="24" t="s">
+      <c r="J75" s="23" t="s">
         <v>343</v>
       </c>
     </row>
@@ -4153,7 +4305,7 @@
       <c r="G80" s="10"/>
       <c r="H80" s="10"/>
     </row>
-    <row r="81" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A81" s="7">
         <v>80</v>
       </c>
@@ -4171,7 +4323,7 @@
       </c>
       <c r="H81" s="10"/>
     </row>
-    <row r="82" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A82" s="7">
         <v>81</v>
       </c>
@@ -4185,7 +4337,7 @@
       <c r="G82" s="10"/>
       <c r="H82" s="10"/>
     </row>
-    <row r="83" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A83" s="7">
         <v>82</v>
       </c>
@@ -4207,7 +4359,7 @@
       </c>
       <c r="H83" s="10"/>
     </row>
-    <row r="84" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A84" s="7">
         <v>83</v>
       </c>
@@ -4221,7 +4373,7 @@
       <c r="G84" s="9"/>
       <c r="H84" s="8"/>
     </row>
-    <row r="85" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A85" s="7">
         <v>84</v>
       </c>
@@ -4245,7 +4397,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="86" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A86" s="7">
         <v>85</v>
       </c>
@@ -4261,7 +4413,7 @@
       <c r="G86" s="9"/>
       <c r="H86" s="8"/>
     </row>
-    <row r="87" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A87" s="7">
         <v>86</v>
       </c>
@@ -4285,35 +4437,48 @@
         <v>311</v>
       </c>
     </row>
-    <row r="88" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A88" s="7">
         <v>87</v>
       </c>
       <c r="B88" s="20" t="s">
         <v>312</v>
       </c>
-      <c r="C88" s="2"/>
+      <c r="C88" s="2" t="s">
+        <v>163</v>
+      </c>
       <c r="D88" s="10"/>
       <c r="E88" s="10"/>
       <c r="F88" s="10"/>
       <c r="G88" s="10"/>
       <c r="H88" s="5"/>
-    </row>
-    <row r="89" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I88" t="s">
+        <v>353</v>
+      </c>
+      <c r="J88" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A89" s="7">
         <v>88</v>
       </c>
       <c r="B89" s="19" t="s">
         <v>313</v>
       </c>
-      <c r="C89" s="2"/>
+      <c r="C89" s="2" t="s">
+        <v>163</v>
+      </c>
       <c r="D89" s="10"/>
       <c r="E89" s="10"/>
       <c r="F89" s="10"/>
       <c r="G89" s="10"/>
       <c r="H89" s="5"/>
-    </row>
-    <row r="90" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J89" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A90" s="7">
         <v>89</v>
       </c>
@@ -4329,7 +4494,7 @@
       <c r="G90" s="10"/>
       <c r="H90" s="5"/>
     </row>
-    <row r="91" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A91" s="7">
         <v>90</v>
       </c>
@@ -4345,7 +4510,7 @@
       <c r="G91" s="10"/>
       <c r="H91" s="5"/>
     </row>
-    <row r="92" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A92" s="7">
         <v>91</v>
       </c>
@@ -4361,7 +4526,7 @@
       <c r="G92" s="10"/>
       <c r="H92" s="5"/>
     </row>
-    <row r="93" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A93" s="7">
         <v>92</v>
       </c>
@@ -4377,7 +4542,7 @@
       <c r="G93" s="10"/>
       <c r="H93" s="5"/>
     </row>
-    <row r="94" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A94" s="7">
         <v>93</v>
       </c>
@@ -4393,7 +4558,7 @@
       <c r="G94" s="10"/>
       <c r="H94" s="5"/>
     </row>
-    <row r="95" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A95" s="7">
         <v>94</v>
       </c>
@@ -4409,7 +4574,7 @@
       <c r="G95" s="10"/>
       <c r="H95" s="5"/>
     </row>
-    <row r="96" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A96" s="7">
         <v>95</v>
       </c>
@@ -4521,7 +4686,7 @@
         <v>327</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>274</v>
+        <v>163</v>
       </c>
       <c r="D102" s="10"/>
       <c r="E102" s="10"/>
@@ -4537,7 +4702,7 @@
         <v>328</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>274</v>
+        <v>163</v>
       </c>
       <c r="D103" s="10"/>
       <c r="E103" s="10"/>
@@ -4553,7 +4718,7 @@
         <v>329</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>274</v>
+        <v>163</v>
       </c>
       <c r="D104" s="10"/>
       <c r="E104" s="10"/>
@@ -4569,7 +4734,7 @@
         <v>330</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>274</v>
+        <v>163</v>
       </c>
       <c r="D105" s="10"/>
       <c r="E105" s="10"/>
@@ -4585,7 +4750,7 @@
         <v>331</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>274</v>
+        <v>163</v>
       </c>
       <c r="D106" s="10"/>
       <c r="E106" s="10"/>
@@ -4601,7 +4766,7 @@
         <v>332</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>274</v>
+        <v>163</v>
       </c>
       <c r="D107" s="10"/>
       <c r="E107" s="10"/>
@@ -4617,7 +4782,7 @@
         <v>333</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>274</v>
+        <v>163</v>
       </c>
       <c r="D108" s="10"/>
       <c r="E108" s="10"/>

</xml_diff>